<commit_message>
finish befor holiday kinda work, need to verify the compute month (weird coding/ due to the merging)
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6015" yWindow="1980" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="31575" yWindow="2235" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tool" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,8 +16,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="7">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0\ \€"/>
+    <numFmt numFmtId="165" formatCode="0 €"/>
+    <numFmt numFmtId="166" formatCode="0 \%"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -42,22 +46,15 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF9C6500"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
@@ -66,8 +63,21 @@
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF006100"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -82,16 +92,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -111,8 +111,42 @@
         <bgColor rgb="FFDA9694"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3E5FC"/>
+        <bgColor rgb="FFB3E5FC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B8E6FF"/>
+        <bgColor rgb="00B8E6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B8FFD1"/>
+        <bgColor rgb="00B8FFD1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -136,6 +170,34 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -152,30 +214,105 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -201,73 +338,76 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thick"/>
+      <right style="thin"/>
+      <top style="thick"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thick"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thick"/>
+      <top style="thin"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="20" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -275,49 +415,116 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="6">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" pivotButton="0" quotePrefix="0" xfId="5"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="9">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" pivotButton="0" quotePrefix="0" xfId="10"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="11">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="11" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="11">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="11" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="11">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="12">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="12" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="12">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="12" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="12">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="10">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Entrée" xfId="2" builtinId="20"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
-    <cellStyle name="Neutre" xfId="4" builtinId="28"/>
-    <cellStyle name="Sortie" xfId="5" builtinId="21"/>
-    <cellStyle name="style_cat1" xfId="6"/>
-    <cellStyle name="style_cat2" xfId="7"/>
-    <cellStyle name="Input" xfId="8" builtinId="20" hidden="0"/>
-    <cellStyle name="Neutral" xfId="9" builtinId="28" hidden="0"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" hidden="0"/>
+    <cellStyle name="Sortie" xfId="3" builtinId="21"/>
+    <cellStyle name="style_cat1" xfId="4"/>
+    <cellStyle name="style_cat2" xfId="5"/>
+    <cellStyle name="Note" xfId="6" builtinId="10"/>
+    <cellStyle name="style_title" xfId="7"/>
+    <cellStyle name="style_title_val" xfId="8"/>
+    <cellStyle name="Satisfaisant" xfId="9" builtinId="26"/>
+    <cellStyle name="Good" xfId="10" builtinId="26" hidden="0"/>
+    <cellStyle name="style_cat7" xfId="11" hidden="0"/>
+    <cellStyle name="style_cat6" xfId="12" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -683,24 +890,24 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" style="8" min="1" max="1"/>
-    <col width="15" customWidth="1" style="8" min="2" max="4"/>
+    <col width="22" customWidth="1" style="20" min="1" max="1"/>
+    <col width="15" customWidth="1" style="20" min="2" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="8">
-      <c r="A1" s="7" t="inlineStr">
+    <row r="1" ht="15.75" customHeight="1" s="20">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>Solde d'initialisation</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>Mai</t>
+      <c r="B1" s="19" t="inlineStr">
+        <is>
+          <t>mai</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
@@ -714,8 +921,11 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" s="8">
-      <c r="A2" s="7" t="n"/>
+    <row r="2" ht="15.75" customHeight="1" s="20">
+      <c r="A2" s="17" t="n">
+        <v>500</v>
+      </c>
+      <c r="B2" s="18" t="n"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>Abonnement</t>
@@ -932,6 +1142,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
@@ -945,25 +1156,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="34" customWidth="1" style="8" min="1" max="1"/>
-    <col width="16" customWidth="1" style="8" min="2" max="2"/>
-    <col width="26" customWidth="1" style="8" min="3" max="3"/>
-    <col width="11" customWidth="1" style="8" min="4" max="4"/>
-    <col width="2" customWidth="1" style="8" min="5" max="5"/>
-    <col width="20" customWidth="1" style="8" min="6" max="6"/>
-    <col width="20" customWidth="1" style="8" min="7" max="7"/>
-    <col width="20" customWidth="1" style="8" min="8" max="8"/>
-    <col width="20" customWidth="1" style="8" min="9" max="9"/>
-    <col width="15" customWidth="1" style="8" min="10" max="10"/>
-    <col width="15" customWidth="1" style="8" min="11" max="11"/>
+    <col width="34" customWidth="1" style="20" min="1" max="1"/>
+    <col width="16" customWidth="1" style="20" min="2" max="2"/>
+    <col width="26" customWidth="1" style="20" min="3" max="3"/>
+    <col width="11" customWidth="1" style="20" min="4" max="4"/>
+    <col width="2" customWidth="1" style="20" min="5" max="5"/>
+    <col width="20" customWidth="1" style="20" min="6" max="9"/>
+    <col width="15" customWidth="1" style="20" min="10" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -973,270 +1180,415 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Solde précédent: 500 (mai)</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
-      <c r="A3" s="16" t="inlineStr">
+      <c r="A3" s="19" t="inlineStr">
         <is>
           <t>#juin</t>
         </is>
       </c>
-    </row>
-    <row r="4"/>
-    <row r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="4" t="n"/>
-      <c r="C5" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>Total transaction</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>Dépense totale</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>Revenue totale</t>
+        </is>
+      </c>
+      <c r="I3" s="22" t="inlineStr">
+        <is>
+          <t>Total réelle</t>
+        </is>
+      </c>
+      <c r="J3" s="23" t="inlineStr">
+        <is>
+          <t>Dépense réelle</t>
+        </is>
+      </c>
+      <c r="K3" s="24" t="inlineStr">
+        <is>
+          <t>Revenue réel</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" s="6" t="n">
+        <v>404.7</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>-1174.9</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>1579.6</v>
+      </c>
+      <c r="I4" s="25" t="n">
+        <v>404.7</v>
+      </c>
+      <c r="J4" s="26" t="n">
+        <v>-1174.9</v>
+      </c>
+      <c r="K4" s="27" t="n">
+        <v>1579.6</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" s="20">
+      <c r="A5" s="7" t="n"/>
+      <c r="B5" s="8" t="n"/>
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">THALES AVS FRANCE SAS </t>
         </is>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="4" t="n">
         <v>1388.58</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3" t="n"/>
-      <c r="B6" s="4" t="n"/>
-      <c r="C6" t="inlineStr">
+    <row r="6" ht="15.75" customHeight="1" s="20">
+      <c r="A6" s="7" t="n"/>
+      <c r="B6" s="8" t="n"/>
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">LAVERIE DES AL </t>
         </is>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="4" t="n">
         <v>-4.5</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="n"/>
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" t="inlineStr">
+      <c r="F6" s="28" t="inlineStr">
+        <is>
+          <t>zz</t>
+        </is>
+      </c>
+      <c r="G6" s="28" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H6" s="29" t="n">
+        <v>-538</v>
+      </c>
+      <c r="I6" s="30" t="n">
+        <v>45.79</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" s="20">
+      <c r="A7" s="7" t="n"/>
+      <c r="B7" s="8" t="n"/>
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">FLIX </t>
         </is>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="4" t="n">
         <v>-24.96</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" t="inlineStr">
+      <c r="F7" s="28" t="inlineStr">
+        <is>
+          <t>zaza</t>
+        </is>
+      </c>
+      <c r="G7" s="28" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H7" s="29" t="n">
+        <v>-177.6</v>
+      </c>
+      <c r="I7" s="30" t="n">
+        <v>15.12</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" s="20">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="8" t="n"/>
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AMAZON PAYMENT </t>
         </is>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="4" t="n">
         <v>-66.55</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="n"/>
-      <c r="B9" s="4" t="n"/>
-      <c r="C9" t="inlineStr">
+      <c r="F8" s="31" t="inlineStr">
+        <is>
+          <t>aza</t>
+        </is>
+      </c>
+      <c r="G8" s="31" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H8" s="32" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="I8" s="33" t="n">
+        <v>9.359999999999999</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" s="20">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>aza</t>
+        </is>
+      </c>
+      <c r="B9" s="8" t="n"/>
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">CAF DE LA DROME </t>
         </is>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="4" t="n">
         <v>191</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="n"/>
-      <c r="B10" s="4" t="n"/>
-      <c r="C10" t="inlineStr">
+    <row r="10" ht="15.75" customHeight="1" s="20">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>aza</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="n"/>
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">LIDL </t>
         </is>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="4" t="n">
         <v>-43.12</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3" t="n"/>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" t="inlineStr">
+    <row r="11" ht="15.75" customHeight="1" s="20">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>zz</t>
+        </is>
+      </c>
+      <c r="B11" s="8" t="n"/>
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SARL RESIDENCE IRINA </t>
         </is>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="4" t="n">
         <v>-520</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" t="inlineStr">
+    <row r="12" ht="15.75" customHeight="1" s="20">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>zz</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="n"/>
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">DROME TEA </t>
         </is>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="4" t="n">
         <v>-18</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3" t="n"/>
-      <c r="B13" s="4" t="n"/>
-      <c r="C13" t="inlineStr">
+    <row r="13" ht="15.75" customHeight="1" s="20">
+      <c r="A13" s="7" t="n"/>
+      <c r="B13" s="8" t="n"/>
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SERVICE NAVIGO </t>
         </is>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="4" t="n">
         <v>-11.15</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="3" t="n"/>
-      <c r="B14" s="4" t="n"/>
-      <c r="C14" t="inlineStr">
+    <row r="14" ht="15.75" customHeight="1" s="20">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>zaza</t>
+        </is>
+      </c>
+      <c r="B14" s="8" t="n"/>
+      <c r="C14" s="3" t="inlineStr">
         <is>
           <t>Revolut</t>
         </is>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="4" t="n">
         <v>-160</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="3" t="n"/>
-      <c r="B15" s="4" t="n"/>
-      <c r="C15" t="inlineStr">
+    <row r="15" ht="15.75" customHeight="1" s="20">
+      <c r="A15" s="7" t="n"/>
+      <c r="B15" s="8" t="n"/>
+      <c r="C15" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">LYDIA APP </t>
         </is>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="4" t="n">
         <v>-36</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="3" t="n"/>
-      <c r="B16" s="4" t="n"/>
-      <c r="C16" t="inlineStr">
+    <row r="16" ht="15.75" customHeight="1" s="20">
+      <c r="A16" s="7" t="n"/>
+      <c r="B16" s="8" t="n"/>
+      <c r="C16" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">COMPASS GROUP </t>
         </is>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" s="4" t="n">
         <v>-70</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="3" t="n"/>
-      <c r="B17" s="4" t="n"/>
-      <c r="C17" t="inlineStr">
+    <row r="17" ht="15.75" customHeight="1" s="20">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>zaza</t>
+        </is>
+      </c>
+      <c r="B17" s="8" t="n"/>
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">PEAGE AUTOROUT </t>
         </is>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" s="4" t="n">
         <v>-17.6</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="3" t="n"/>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" t="inlineStr">
+    <row r="18" ht="15.75" customHeight="1" s="20">
+      <c r="A18" s="7" t="n"/>
+      <c r="B18" s="8" t="n"/>
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SPYROJANNOPOUL </t>
         </is>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" s="4" t="n">
         <v>-55</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="3" t="n"/>
-      <c r="B19" s="4" t="n"/>
-      <c r="C19" t="inlineStr">
+    <row r="19" ht="15.75" customHeight="1" s="20">
+      <c r="A19" s="7" t="n"/>
+      <c r="B19" s="8" t="n"/>
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>Spotify P</t>
         </is>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="4" t="n">
         <v>-5.99</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="3" t="n"/>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" t="inlineStr">
+    <row r="20" ht="15.75" customHeight="1" s="20">
+      <c r="A20" s="7" t="n"/>
+      <c r="B20" s="8" t="n"/>
+      <c r="C20" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SNCF INTERNET </t>
         </is>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" s="4" t="n">
         <v>-107</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="3" t="n"/>
-      <c r="B21" s="4" t="n"/>
-      <c r="C21" t="inlineStr">
+    <row r="21" ht="15.75" customHeight="1" s="20">
+      <c r="A21" s="7" t="n"/>
+      <c r="B21" s="8" t="n"/>
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">BASIC FIT II SA </t>
         </is>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" s="4" t="n">
         <v>-34.98</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="3" t="n"/>
-      <c r="B22" s="4" t="n"/>
-      <c r="D22" s="5" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="n"/>
-      <c r="B23" s="4" t="n"/>
-      <c r="D23" s="5" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="n"/>
-      <c r="B24" s="4" t="n"/>
-      <c r="D24" s="5" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="3" t="n"/>
-      <c r="B25" s="4" t="n"/>
-      <c r="D25" s="5" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="n"/>
-      <c r="B26" s="4" t="n"/>
-      <c r="D26" s="5" t="n"/>
-    </row>
-    <row r="27">
+    <row r="22" ht="15.75" customHeight="1" s="20">
+      <c r="A22" s="7" t="n"/>
+      <c r="B22" s="8" t="n"/>
+      <c r="C22" s="3" t="n"/>
+      <c r="D22" s="4" t="n"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" s="20">
+      <c r="A23" s="7" t="n"/>
+      <c r="B23" s="8" t="n"/>
+      <c r="C23" s="3" t="n"/>
+      <c r="D23" s="4" t="n"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" s="20">
+      <c r="A24" s="7" t="n"/>
+      <c r="B24" s="8" t="n"/>
+      <c r="C24" s="3" t="n"/>
+      <c r="D24" s="4" t="n"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" s="20">
+      <c r="A25" s="7" t="n"/>
+      <c r="B25" s="8" t="n"/>
+      <c r="C25" s="3" t="n"/>
+      <c r="D25" s="4" t="n"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1" s="20">
+      <c r="A26" s="7" t="n"/>
+      <c r="B26" s="8" t="n"/>
+      <c r="C26" s="3" t="n"/>
+      <c r="D26" s="4" t="n"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1" s="20">
       <c r="A27" t="inlineStr">
         <is>
           <t>&gt;solde fiche de paye (fin du mois)</t>
         </is>
       </c>
-      <c r="B27" s="5" t="n"/>
-      <c r="C27" s="17" t="inlineStr">
+      <c r="B27" s="9" t="n">
+        <v>904</v>
+      </c>
+      <c r="C27" s="34" t="inlineStr">
         <is>
           <t>Verif</t>
         </is>
       </c>
-      <c r="D27" s="17" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="18" t="inlineStr">
+      <c r="D27" s="34" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" s="20">
+      <c r="A28" s="10" t="inlineStr">
         <is>
           <t>Solde estimé :</t>
         </is>
       </c>
-      <c r="B28" s="18" t="n"/>
+      <c r="B28" s="10" t="n">
+        <v>904.73</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
+  <mergeCells count="6">
     <mergeCell ref="A3:D4"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F6"/>
+    <mergeCell ref="F7"/>
+    <mergeCell ref="F8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>